<commit_message>
Refactor SimObject_Metadata and related schemas; enhance settings sanitization and validation tests for ACTIVE_METADATA. Remove yaml_to_simobject_metadata
</commit_message>
<xml_diff>
--- a/test_e2e/main-treasury-temp/engine_settings_sanitization_set/data.xlsx
+++ b/test_e2e/main-treasury-temp/engine_settings_sanitization_set/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\e3\@gitwk\PUBLIC\financial-modeling\test_e2e\main-treasury-temp\engine_settings_sanitization_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED54F410-CFD8-46A2-AF3E-9946D2788284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A585E781-DCC8-46FF-B6D1-F0C71B40944E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E11AB095-19A6-4A4D-A920-1BEA7BE72FFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>$</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>{mamma: ines, babbo: loreto}</t>
+  </si>
+  <si>
+    <t>ACTIVE_METADATA</t>
+  </si>
+  <si>
+    <t>{ name: [AA, AAA], value: [BB, BBB], weight: [0.5, 0.6] }</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D686B419-447E-48DA-BE72-2964E26B0617}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -530,6 +536,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>